<commit_message>
[XAMPP Setup for Wordpress] 회사 mytheme 계정정보 update
</commit_message>
<xml_diff>
--- a/XAMPP Setup for Wordpress.xlsx
+++ b/XAMPP Setup for Wordpress.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="670" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="670" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="계정" sheetId="9" r:id="rId1"/>
@@ -15,13 +15,14 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'wordpress Setup'!$A$1:$P$136</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'xampp Setup'!$A$1:$Q$199</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">계정!$A$1:$I$39</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="57">
   <si>
     <t>9. 데이터베이스 tap에서 동일 계정으로 데이터베이스가 생성됐는지 확인한다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -220,6 +221,34 @@
   </si>
   <si>
     <t>mytheme</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Position</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Site</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Home</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Company</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wp_mytheme</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mytheme</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wp1234</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -227,7 +256,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -259,16 +288,31 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -276,19 +320,287 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -299,6 +611,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1338,8 +1653,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="832340" y="734891"/>
-          <a:ext cx="6194180" cy="1846584"/>
+          <a:off x="840504" y="725366"/>
+          <a:ext cx="6145195" cy="1797598"/>
           <a:chOff x="849925" y="710713"/>
           <a:chExt cx="6220557" cy="1872961"/>
         </a:xfrm>
@@ -1453,8 +1768,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="832337" y="3234836"/>
-          <a:ext cx="7329828" cy="2403231"/>
+          <a:off x="840501" y="3159997"/>
+          <a:ext cx="7275400" cy="2343359"/>
           <a:chOff x="835268" y="3275134"/>
           <a:chExt cx="7359135" cy="2435470"/>
         </a:xfrm>
@@ -1614,8 +1929,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="794236" y="6376085"/>
-          <a:ext cx="8190037" cy="4090173"/>
+          <a:off x="802400" y="6219603"/>
+          <a:ext cx="8130166" cy="3986759"/>
           <a:chOff x="797167" y="6460345"/>
           <a:chExt cx="8222275" cy="4145857"/>
         </a:xfrm>
@@ -1775,8 +2090,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="876301" y="11285659"/>
-          <a:ext cx="4664320" cy="2463365"/>
+          <a:off x="884465" y="11003991"/>
+          <a:ext cx="4631663" cy="2398051"/>
           <a:chOff x="886559" y="11136923"/>
           <a:chExt cx="4681904" cy="2498535"/>
         </a:xfrm>
@@ -2028,8 +2343,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="825011" y="14149817"/>
-          <a:ext cx="7453680" cy="1994325"/>
+          <a:off x="833175" y="13791949"/>
+          <a:ext cx="7399252" cy="1945339"/>
           <a:chOff x="827942" y="14342515"/>
           <a:chExt cx="7482987" cy="2020702"/>
         </a:xfrm>
@@ -2204,8 +2519,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="825012" y="17123751"/>
-          <a:ext cx="5530361" cy="5257790"/>
+          <a:off x="833176" y="16689683"/>
+          <a:ext cx="5486818" cy="5121719"/>
           <a:chOff x="827943" y="17357480"/>
           <a:chExt cx="5553807" cy="5331059"/>
         </a:xfrm>
@@ -2966,7 +3281,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3001,7 +3316,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3210,101 +3525,311 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G7"/>
+  <dimension ref="B2:I25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7:G7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.25" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.625" customWidth="1"/>
+    <col min="2" max="2" width="14.75" customWidth="1"/>
+    <col min="3" max="3" width="21.25" customWidth="1"/>
+    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5" customWidth="1"/>
+    <col min="7" max="7" width="12.625" customWidth="1"/>
+    <col min="8" max="8" width="16.625" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B2" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C4" s="4" t="s">
+    <row r="3" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B4" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="22"/>
+      <c r="F4" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C5" t="s">
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="23"/>
+    </row>
+    <row r="5" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="24"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" s="26" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
+      <c r="I5" s="27"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B6" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" s="18" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+      <c r="I6" s="19"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B7" s="7"/>
+      <c r="C7" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" s="8" t="s">
         <v>47</v>
       </c>
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B8" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B9" s="10"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B10" s="10"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="6"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B11" s="10"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="10"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="6"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B13" s="10"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="10"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="6"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B15" s="10"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="6"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B16" s="10"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="6"/>
+    </row>
+    <row r="17" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="11"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="13"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:G4"/>
+  <mergeCells count="5">
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3312,7 +3837,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D138"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A32" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A80" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
@@ -3423,8 +3948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A97" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <selection activeCell="M108" sqref="M108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3510,7 +4035,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C74"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N51" sqref="N51"/>
     </sheetView>
   </sheetViews>

</xml_diff>